<commit_message>
Corrected the excel files
</commit_message>
<xml_diff>
--- a/Setup/LoadDimensions_human.xlsx
+++ b/Setup/LoadDimensions_human.xlsx
@@ -29,31 +29,31 @@
     <t>Name</t>
   </si>
   <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>1.61 to 1.56</t>
+  </si>
+  <si>
+    <t>0.24 to 0.23</t>
+  </si>
+  <si>
+    <t>short edge</t>
+  </si>
+  <si>
+    <t>long edge</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
     <t>width</t>
-  </si>
-  <si>
-    <t>height</t>
-  </si>
-  <si>
-    <t>thickness</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>1.61 to 1.56</t>
-  </si>
-  <si>
-    <t>0.24 to 0.23</t>
-  </si>
-  <si>
-    <t>short edge</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -395,21 +395,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>0.80500000000000005</v>
@@ -424,12 +424,12 @@
         <v>0.40500000000000003</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>1.59</v>
@@ -444,12 +444,12 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>3.2</v>

</xml_diff>